<commit_message>
Updates FHIR resource urls and FSH aliases
</commit_message>
<xml_diff>
--- a/output/CodeSystem-q4ms-anfragekategorie.xlsx
+++ b/output/CodeSystem-q4ms-anfragekategorie.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://qpath.ukdd.de/CodeSystem/q4ms-anfragekategorie</t>
+    <t>http://terminology-fgdh.wiwi.tu-dresden.de/fhir/CodeSystem/q4ms-anfragekategorie</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-22T11:59:55+01:00</t>
+    <t>2021-12-22T13:43:58+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Fixes some url issues and santitize titles
</commit_message>
<xml_diff>
--- a/output/CodeSystem-q4ms-anfragekategorie.xlsx
+++ b/output/CodeSystem-q4ms-anfragekategorie.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Anfragekategorie CodeSystem</t>
+    <t>Anfragekategorie</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-22T13:43:58+01:00</t>
+    <t>2021-12-22T19:56:03+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Updates IG sushi configuration
</commit_message>
<xml_diff>
--- a/output/CodeSystem-q4ms-anfragekategorie.xlsx
+++ b/output/CodeSystem-q4ms-anfragekategorie.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>Property</t>
   </si>
@@ -57,19 +57,25 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-22T19:56:03+01:00</t>
+    <t>2021-12-22T21:26:07+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>QPath4MS</t>
+    <t>Forschungsgruppe Digital Health</t>
   </si>
   <si>
     <t>Contact</t>
   </si>
   <si>
     <t>No display for ContactDetail</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
   <si>
     <t>Description</t>
@@ -323,7 +329,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -413,43 +419,47 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B14" t="s" s="2">
-        <v>24</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
@@ -467,22 +477,34 @@
       <c r="A19" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="B19" t="s" s="2">
-        <v>30</v>
-      </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="B21" t="s" s="2">
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
         <v>33</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -500,114 +522,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s" s="2">
         <v>46</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unifies IG's canonical urls and adds terminology publishing script
</commit_message>
<xml_diff>
--- a/output/CodeSystem-q4ms-anfragekategorie.xlsx
+++ b/output/CodeSystem-q4ms-anfragekategorie.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://terminology-fgdh.wiwi.tu-dresden.de/fhir/CodeSystem/q4ms-anfragekategorie</t>
+    <t>http://qpath4ms.ukdd.de/fhir/CodeSystem/q4ms-anfragekategorie</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-22T21:26:07+01:00</t>
+    <t>2022-01-03T16:30:59+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>